<commit_message>
fixed data parsing for edge cases
</commit_message>
<xml_diff>
--- a/tests/WebVella.Tefter.DataProviders.Excel.Tests/Files/data.xlsx
+++ b/tests/WebVella.Tefter.DataProviders.Excel.Tests/Files/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\sample-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\WebVella.Tefter\tests\WebVella.Tefter.DataProviders.Excel.Tests\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C9A8B-A566-44BD-8149-814786413442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57640DD9-F21C-4DBC-B69A-AB996EB41606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12612" yWindow="5976" windowWidth="33744" windowHeight="18792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57465" yWindow="9075" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -129,7 +129,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>